<commit_message>
Degree of freedom correction for clustered EPA
</commit_message>
<xml_diff>
--- a/Results/results_clustered.xlsx
+++ b/Results/results_clustered.xlsx
@@ -12,17 +12,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">T</t>
+    <t xml:space="preserve">Tobs</t>
   </si>
   <si>
     <t xml:space="preserve">d</t>
   </si>
   <si>
+    <t xml:space="preserve">variant</t>
+  </si>
+  <si>
     <t xml:space="preserve">known</t>
   </si>
   <si>
@@ -45,6 +48,15 @@
   </si>
   <si>
     <t xml:space="preserve">selective_cond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selective_mode2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selective_mode2_cond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overall_holds</t>
   </si>
 </sst>
 </file>
@@ -410,6 +422,15 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -421,29 +442,170 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.054</v>
       </c>
-      <c r="E2" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>80</v>
+      </c>
+      <c r="B3" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.06</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K3" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="M3" t="n">
         <v>0.064</v>
       </c>
-      <c r="K2" t="n">
-        <v>0.052</v>
+      <c r="N3" t="n">
+        <v>0.049</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>80</v>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.029</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>80</v>
+      </c>
+      <c r="B5" t="n">
+        <v>200</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>